<commit_message>
Minor changes to instructors' students view
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -3078,7 +3078,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -3941,7 +3941,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -3968,7 +3968,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="29" customWidth="1" min="1" max="1"/>
-    <col width="48" customWidth="1" min="2" max="2"/>
+    <col width="57" customWidth="1" min="2" max="2"/>
     <col width="9.15" customWidth="1" min="3" max="3"/>
     <col width="9.15" customWidth="1" min="4" max="4"/>
     <col width="11" customWidth="1" min="5" max="5"/>
@@ -4015,11 +4015,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>GEE12D-M, CS413-M, CC413-M, GEE12D-M, GEE11D-M</t>
+          <t>GEE12D-M, CS413-M, CS413-M, CC413-M, GEE12D-M, GEE11D-M</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -4028,7 +4028,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -4279,7 +4279,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -4288,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Functionality and UI updates
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -1185,12 +1185,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Age'!$A$2:$A$5</f>
+              <f>'Age'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Age'!$B$2:$B$5</f>
+              <f>'Age'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -1433,12 +1433,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Faculty - Subjects'!$A$2:$A$6</f>
+              <f>'Faculty - Subjects'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Faculty - Subjects'!$B$2:$B$6</f>
+              <f>'Faculty - Subjects'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -1457,12 +1457,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Faculty - Subjects'!$A$2:$A$6</f>
+              <f>'Faculty - Subjects'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Faculty - Subjects'!$C$2:$C$6</f>
+              <f>'Faculty - Subjects'!$C$2:$C$7</f>
             </numRef>
           </val>
         </ser>
@@ -1481,12 +1481,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Faculty - Subjects'!$A$2:$A$6</f>
+              <f>'Faculty - Subjects'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Faculty - Subjects'!$D$2:$D$6</f>
+              <f>'Faculty - Subjects'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -1505,12 +1505,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Faculty - Subjects'!$A$2:$A$6</f>
+              <f>'Faculty - Subjects'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Faculty - Subjects'!$E$2:$E$6</f>
+              <f>'Faculty - Subjects'!$E$2:$E$7</f>
             </numRef>
           </val>
         </ser>
@@ -1529,12 +1529,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Faculty - Subjects'!$A$2:$A$6</f>
+              <f>'Faculty - Subjects'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Faculty - Subjects'!$F$2:$F$6</f>
+              <f>'Faculty - Subjects'!$F$2:$F$7</f>
             </numRef>
           </val>
         </ser>
@@ -1641,12 +1641,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Student - Subjects'!$A$2:$A$8</f>
+              <f>'Student - Subjects'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Student - Subjects'!$B$2:$B$8</f>
+              <f>'Student - Subjects'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -1665,12 +1665,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Student - Subjects'!$A$2:$A$8</f>
+              <f>'Student - Subjects'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Student - Subjects'!$C$2:$C$8</f>
+              <f>'Student - Subjects'!$C$2:$C$9</f>
             </numRef>
           </val>
         </ser>
@@ -1689,12 +1689,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Student - Subjects'!$A$2:$A$8</f>
+              <f>'Student - Subjects'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Student - Subjects'!$D$2:$D$8</f>
+              <f>'Student - Subjects'!$D$2:$D$9</f>
             </numRef>
           </val>
         </ser>
@@ -1713,12 +1713,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Student - Subjects'!$A$2:$A$8</f>
+              <f>'Student - Subjects'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Student - Subjects'!$E$2:$E$8</f>
+              <f>'Student - Subjects'!$E$2:$E$9</f>
             </numRef>
           </val>
         </ser>
@@ -2676,7 +2676,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -3078,7 +3078,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -3624,7 +3624,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -3789,7 +3789,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3846,10 +3846,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>2024-2nd-22</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>2024-2nd-23</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3944,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3959,7 +3969,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4123,6 +4133,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dolores Montesines </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -4135,7 +4165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4307,6 +4337,25 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cruz KC </t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4398,7 +4447,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>

</xml_diff>